<commit_message>
Get TP, TN, FP, FN for all relevant models
</commit_message>
<xml_diff>
--- a/results/All variables without tuition with_cv_1.xlsx
+++ b/results/All variables without tuition with_cv_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Model</t>
   </si>
@@ -34,22 +34,7 @@
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Lasso</t>
-  </si>
-  <si>
-    <t>Support Vector Classifier</t>
-  </si>
-  <si>
-    <t>CART</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
     <t>LightGBM</t>
-  </si>
-  <si>
-    <t>XGBoost</t>
   </si>
 </sst>
 </file>
@@ -407,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,16 +420,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.903030303030303</v>
+        <v>0.9033057851239669</v>
       </c>
       <c r="C2">
-        <v>0.9041563072876582</v>
+        <v>0.9044857886687019</v>
       </c>
       <c r="D2">
-        <v>0.903030303030303</v>
+        <v>0.9033057851239669</v>
       </c>
       <c r="E2">
-        <v>0.9019821835816357</v>
+        <v>0.9022504752972083</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -452,101 +437,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.9002754820936639</v>
+        <v>0.9005509641873278</v>
       </c>
       <c r="C3">
-        <v>0.9009459442048033</v>
+        <v>0.901507456759959</v>
       </c>
       <c r="D3">
-        <v>0.9002754820936639</v>
+        <v>0.9005509641873278</v>
       </c>
       <c r="E3">
-        <v>0.8994200359756892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0.8865013774104684</v>
-      </c>
-      <c r="C4">
-        <v>0.8915337247464443</v>
-      </c>
-      <c r="D4">
-        <v>0.8865013774104684</v>
-      </c>
-      <c r="E4">
-        <v>0.884164359417559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0.8509641873278238</v>
-      </c>
-      <c r="C5">
-        <v>0.8520002469976624</v>
-      </c>
-      <c r="D5">
-        <v>0.8509641873278238</v>
-      </c>
-      <c r="E5">
-        <v>0.8511282082838815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>0.8922865013774104</v>
-      </c>
-      <c r="C6">
-        <v>0.8938656685776083</v>
-      </c>
-      <c r="D6">
-        <v>0.8922865013774104</v>
-      </c>
-      <c r="E6">
-        <v>0.8909191366117082</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0.9005509641873278</v>
-      </c>
-      <c r="C7">
-        <v>0.901507456759959</v>
-      </c>
-      <c r="D7">
-        <v>0.9005509641873278</v>
-      </c>
-      <c r="E7">
         <v>0.8995899653084244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.8988980716253444</v>
-      </c>
-      <c r="C8">
-        <v>0.8999594192581993</v>
-      </c>
-      <c r="D8">
-        <v>0.8988980716253444</v>
-      </c>
-      <c r="E8">
-        <v>0.8978401188785023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>